<commit_message>
cierre de 21 AGOSTO
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01 DOCUEMENTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -114,7 +114,7 @@
     <t>.</t>
   </si>
   <si>
-    <t>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</t>
+    <t>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</t>
   </si>
 </sst>
 </file>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="31">
-        <v>0</v>
+        <v>867</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
       <c r="H6" s="7"/>
       <c r="K6" s="23">
         <f>SUM(K3:K5)</f>
-        <v>2600</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="K9" s="24"/>
     </row>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C14" s="42">
         <f ca="1">TODAY()</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="E14" s="24"/>
       <c r="G14" s="6"/>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="I14" s="42">
         <f ca="1">C14</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="K14" s="24"/>
     </row>
@@ -1284,13 +1284,13 @@
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="E27" s="24"/>
       <c r="G27" s="6"/>
       <c r="H27" s="7" t="str">
         <f>B27</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="K27" s="24"/>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C32" s="42">
         <f ca="1">I14</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="E32" s="24"/>
       <c r="G32" s="6"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="I32" s="42">
         <f ca="1">C32</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="K32" s="24"/>
     </row>
@@ -1461,7 +1461,7 @@
         <v>24</v>
       </c>
       <c r="K40" s="41">
-        <v>1042</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:11" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
@@ -1476,7 +1476,7 @@
       <c r="I41" s="40"/>
       <c r="K41" s="23">
         <f>SUM(K38:K40)</f>
-        <v>3042</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
@@ -1489,13 +1489,13 @@
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="str">
         <f>H27</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="E43" s="24"/>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="str">
         <f>B43</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="K43" s="24"/>
     </row>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C48" s="42">
         <f ca="1">C32</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="E48" s="24"/>
       <c r="G48" s="6"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="I48" s="42">
         <f ca="1">C48</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="K48" s="24"/>
     </row>
@@ -1680,7 +1680,7 @@
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">
         <f>H43</f>
-        <v>SEMANA   33  DEL  09  Al    15  AGOSTO         2021</v>
+        <v>SEMANA   34  DEL  16  Al    22  AGOSTO         2021</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="38"/>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C65" s="42">
         <f ca="1">I48</f>
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="E65" s="24"/>
       <c r="F65" s="38"/>

</xml_diff>

<commit_message>
CIERRE 28 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -111,7 +111,7 @@
     <t>.</t>
   </si>
   <si>
-    <t>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</t>
+    <t>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I59" sqref="H59:I59"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="K9" s="24"/>
     </row>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C14" s="42">
         <f ca="1">TODAY()</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="E14" s="24"/>
       <c r="G14" s="6"/>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="I14" s="42">
         <f ca="1">C14</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="K14" s="24"/>
     </row>
@@ -1276,13 +1276,13 @@
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="E27" s="24"/>
       <c r="G27" s="6"/>
       <c r="H27" s="7" t="str">
         <f>B27</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="K27" s="24"/>
     </row>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="C32" s="42">
         <f ca="1">I14</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="E32" s="24"/>
       <c r="G32" s="6"/>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="I32" s="42">
         <f ca="1">C32</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="K32" s="24"/>
     </row>
@@ -1481,13 +1481,13 @@
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="str">
         <f>H27</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="E43" s="24"/>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="str">
         <f>B43</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="K43" s="24"/>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="C48" s="42">
         <f ca="1">C32</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="E48" s="24"/>
       <c r="G48" s="6"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="I48" s="42">
         <f ca="1">C48</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="K48" s="24"/>
     </row>
@@ -1672,7 +1672,7 @@
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">
         <f>H43</f>
-        <v>SEMANA   03  DEL    17      Al   23   DE   E N E R O          202</v>
+        <v>SEMANA   04  DEL    24      Al   30   DE   E N E R O          202</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="38"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C65" s="42">
         <f ca="1">I48</f>
-        <v>44583</v>
+        <v>44589</v>
       </c>
       <c r="E65" s="24"/>
       <c r="F65" s="38"/>

</xml_diff>

<commit_message>
cierre 18 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -111,7 +111,7 @@
     <t>.</t>
   </si>
   <si>
-    <t>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</t>
+    <t>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,10 +989,10 @@
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="J3" s="22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K3" s="30">
-        <v>2600</v>
+        <v>867</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1013,7 +1013,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="31">
-        <v>867</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1045,7 +1045,7 @@
       <c r="H6" s="7"/>
       <c r="K6" s="23">
         <f>SUM(K3:K5)</f>
-        <v>3467</v>
+        <v>867</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="K9" s="24"/>
     </row>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="C14" s="42">
         <f ca="1">TODAY()</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="E14" s="24"/>
       <c r="G14" s="6"/>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="I14" s="42">
         <f ca="1">C14</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="K14" s="24"/>
     </row>
@@ -1257,7 +1257,7 @@
         <v>26</v>
       </c>
       <c r="E25" s="17">
-        <v>-283</v>
+        <v>0</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="7"/>
@@ -1267,7 +1267,7 @@
       <c r="B26" s="7"/>
       <c r="E26" s="23">
         <f>SUM(E21:E25)</f>
-        <v>1837.3199999999997</v>
+        <v>2120.3199999999997</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7"/>
@@ -1276,13 +1276,13 @@
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>B9</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="E27" s="24"/>
       <c r="G27" s="6"/>
       <c r="H27" s="7" t="str">
         <f>B27</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="K27" s="24"/>
     </row>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="C32" s="42">
         <f ca="1">I14</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="E32" s="24"/>
       <c r="G32" s="6"/>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="I32" s="42">
         <f ca="1">C32</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="K32" s="24"/>
     </row>
@@ -1479,13 +1479,13 @@
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="str">
         <f>H27</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="E43" s="24"/>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="str">
         <f>B43</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="K43" s="24"/>
     </row>
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C48" s="42">
         <f ca="1">C32</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="E48" s="24"/>
       <c r="G48" s="6"/>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="I48" s="42">
         <f ca="1">C48</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="K48" s="24"/>
     </row>
@@ -1670,7 +1670,7 @@
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">
         <f>H43</f>
-        <v>SEMANA   06  DEL    7      Al   13   DE   FEBRERO          2022</v>
+        <v>SEMANA   07  DEL    14      Al   20   DE   FEBRERO          2022</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="38"/>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="C65" s="42">
         <f ca="1">I48</f>
-        <v>44604</v>
+        <v>44610</v>
       </c>
       <c r="E65" s="24"/>
       <c r="F65" s="38"/>

</xml_diff>

<commit_message>
CIERRE 21 JUL 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -81,7 +81,7 @@
     <t>GUADALUPE LILLO TECOX</t>
   </si>
   <si>
-    <t>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</t>
+    <t>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</t>
   </si>
 </sst>
 </file>
@@ -521,21 +521,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -544,33 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -889,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,7 @@
       <c r="H4" s="7"/>
       <c r="J4" s="39"/>
       <c r="K4" s="14">
-        <v>560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,10 +966,10 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="67"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14">
         <v>0</v>
@@ -984,8 +984,8 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="13"/>
       <c r="K6" s="22">
         <v>0</v>
@@ -1003,7 +1003,7 @@
       <c r="H7" s="7"/>
       <c r="K7" s="42">
         <f>SUM(K4:K6)</f>
-        <v>560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="40" t="str">
         <f>B9</f>
-        <v>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</v>
+        <v>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -1034,30 +1034,30 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="16"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="62"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="62"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="16"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C14" s="29">
         <f ca="1">TODAY()</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="E14" s="15"/>
       <c r="G14" s="6"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="I14" s="29">
         <f ca="1">C14</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="K14" s="15"/>
     </row>
@@ -1173,10 +1173,10 @@
         <v>2800</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="71" t="s">
+      <c r="H23" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="72"/>
+      <c r="I23" s="60"/>
       <c r="J23" s="8">
         <v>6</v>
       </c>
@@ -1185,13 +1185,13 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="32"/>
       <c r="E24" s="31"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
       <c r="J24" s="32"/>
       <c r="K24" s="31"/>
     </row>
@@ -1202,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="28">
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="26"/>
@@ -1219,7 +1219,7 @@
       <c r="C26" s="27"/>
       <c r="E26" s="14">
         <f>SUM(E23:E25)</f>
-        <v>2800</v>
+        <v>4200</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="26"/>
@@ -1239,13 +1239,13 @@
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="40" t="str">
         <f>B9</f>
-        <v>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</v>
+        <v>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</v>
       </c>
       <c r="E28" s="15"/>
       <c r="G28" s="6"/>
       <c r="H28" s="40" t="str">
         <f>B28</f>
-        <v>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</v>
+        <v>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</v>
       </c>
       <c r="K28" s="15"/>
     </row>
@@ -1258,21 +1258,21 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="60"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="66"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="60"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="62"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="68"/>
       <c r="G31" s="6"/>
       <c r="H31" s="7"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="62"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="68"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="C33" s="29">
         <f ca="1">I14</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="E33" s="15"/>
       <c r="G33" s="6"/>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="I33" s="29">
         <f ca="1">C33</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="K33" s="15"/>
     </row>
@@ -1370,10 +1370,10 @@
       <c r="K40" s="21"/>
     </row>
     <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="72"/>
+      <c r="C41" s="60"/>
       <c r="D41" s="8">
         <v>3</v>
       </c>
@@ -1382,10 +1382,10 @@
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="37"/>
-      <c r="H41" s="71" t="s">
+      <c r="H41" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="72"/>
+      <c r="I41" s="60"/>
       <c r="J41" s="8">
         <v>6</v>
       </c>
@@ -1394,14 +1394,14 @@
       </c>
     </row>
     <row r="42" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="32"/>
       <c r="E42" s="31"/>
       <c r="F42" s="12"/>
       <c r="G42" s="37"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
       <c r="J42" s="32"/>
       <c r="K42" s="31"/>
     </row>
@@ -1450,13 +1450,13 @@
     <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="40" t="str">
         <f>H28</f>
-        <v>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</v>
+        <v>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</v>
       </c>
       <c r="E46" s="15"/>
       <c r="G46" s="37"/>
       <c r="H46" s="40" t="str">
         <f>B46</f>
-        <v>SEMANA  28        DEL    10     Al   16  DE   JULIO    2023</v>
+        <v>SEMANA  29        DEL    17     Al   23  DE   JULIO    2023</v>
       </c>
       <c r="K46" s="15"/>
     </row>
@@ -1469,23 +1469,23 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="60"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="66"/>
       <c r="F48" s="16"/>
       <c r="G48" s="37"/>
       <c r="H48" s="7"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="60"/>
+      <c r="J48" s="65"/>
+      <c r="K48" s="66"/>
     </row>
     <row r="49" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="62"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="68"/>
       <c r="F49" s="16"/>
       <c r="G49" s="37"/>
       <c r="H49" s="7"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="62"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="68"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="C51" s="29">
         <f ca="1">C33</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="E51" s="15"/>
       <c r="G51" s="37"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="I51" s="29">
         <f ca="1">I33</f>
-        <v>45121</v>
+        <v>45128</v>
       </c>
       <c r="K51" s="15"/>
     </row>
@@ -1573,20 +1573,20 @@
       <c r="K57" s="46"/>
     </row>
     <row r="58" spans="2:11" s="37" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="71"/>
       <c r="D58" s="52"/>
       <c r="E58" s="48"/>
       <c r="J58" s="47"/>
       <c r="K58" s="48"/>
     </row>
     <row r="59" spans="2:11" s="37" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B59" s="63"/>
-      <c r="C59" s="63"/>
+      <c r="B59" s="72"/>
+      <c r="C59" s="72"/>
       <c r="D59" s="54"/>
       <c r="E59" s="55"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="74"/>
       <c r="J59" s="44"/>
       <c r="K59" s="48"/>
     </row>
@@ -1595,8 +1595,8 @@
       <c r="C60" s="56"/>
       <c r="D60" s="57"/>
       <c r="E60" s="55"/>
-      <c r="H60" s="65"/>
-      <c r="I60" s="65"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="74"/>
       <c r="J60" s="44"/>
       <c r="K60" s="49"/>
     </row>
@@ -1615,16 +1615,16 @@
     </row>
     <row r="64" spans="2:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="64"/>
-      <c r="E65" s="64"/>
-      <c r="J65" s="64"/>
-      <c r="K65" s="64"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73"/>
+      <c r="J65" s="73"/>
+      <c r="K65" s="73"/>
     </row>
     <row r="66" spans="2:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="64"/>
-      <c r="E66" s="64"/>
-      <c r="J66" s="64"/>
-      <c r="K66" s="64"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
+      <c r="J66" s="73"/>
+      <c r="K66" s="73"/>
     </row>
     <row r="67" spans="2:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="2:11" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1637,11 +1637,13 @@
     <row r="70" spans="2:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="J65:K66"/>
+    <mergeCell ref="H59:I60"/>
     <mergeCell ref="H5:I6"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H23:I23"/>
@@ -1650,13 +1652,11 @@
     <mergeCell ref="J11:K12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D30:E31"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="J48:K49"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="J65:K66"/>
-    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 22 SEPT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>RECIBO DE NOMINA</t>
   </si>
@@ -81,10 +81,7 @@
     <t>GUADALUPE LILLO TECOX</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</t>
+    <t>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</t>
   </si>
 </sst>
 </file>
@@ -551,21 +548,48 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -574,33 +598,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -919,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +983,7 @@
       <c r="H4" s="7"/>
       <c r="J4" s="36"/>
       <c r="K4" s="14">
-        <v>0</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -996,10 +993,10 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="74"/>
+      <c r="I5" s="69"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14">
         <v>0</v>
@@ -1014,8 +1011,8 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="76"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
       <c r="J6" s="13"/>
       <c r="K6" s="22">
         <v>0</v>
@@ -1033,7 +1030,7 @@
       <c r="H7" s="7"/>
       <c r="K7" s="39">
         <f>SUM(K4:K6)</f>
-        <v>0</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1045,13 +1042,13 @@
     </row>
     <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="15"/>
       <c r="G9" s="6"/>
       <c r="H9" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</v>
+        <v>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -1064,30 +1061,30 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="16"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="67"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="73"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="69"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="75"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="81"/>
+      <c r="E13" s="77"/>
       <c r="F13" s="16"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
@@ -1105,7 +1102,7 @@
       </c>
       <c r="C14" s="27">
         <f ca="1">TODAY()</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="E14" s="15"/>
       <c r="G14" s="6"/>
@@ -1114,7 +1111,7 @@
       </c>
       <c r="I14" s="27">
         <f ca="1">C14</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="K14" s="15"/>
     </row>
@@ -1203,10 +1200,10 @@
         <v>2800</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="78" t="s">
+      <c r="H23" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="79"/>
+      <c r="I23" s="67"/>
       <c r="J23" s="8">
         <v>6</v>
       </c>
@@ -1215,13 +1212,15 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="30"/>
-      <c r="E24" s="29"/>
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
       <c r="J24" s="30"/>
       <c r="K24" s="29"/>
     </row>
@@ -1232,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="26">
-        <v>0</v>
+        <v>933</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="24"/>
@@ -1247,8 +1246,9 @@
     <row r="26" spans="2:11" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
-      <c r="E26" s="14" t="s">
-        <v>18</v>
+      <c r="E26" s="14">
+        <f>SUM(E22:E25)</f>
+        <v>3733</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="24"/>
@@ -1268,13 +1268,13 @@
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</v>
+        <v>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</v>
       </c>
       <c r="E28" s="15"/>
       <c r="G28" s="6"/>
       <c r="H28" s="37" t="str">
         <f>B28</f>
-        <v>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</v>
+        <v>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</v>
       </c>
       <c r="K28" s="15"/>
     </row>
@@ -1287,21 +1287,21 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="67"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="67"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="73"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="75"/>
       <c r="G31" s="6"/>
       <c r="H31" s="7"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="69"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="75"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C33" s="27">
         <f ca="1">I14</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="E33" s="15"/>
       <c r="G33" s="6"/>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="I33" s="27">
         <f ca="1">C33</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="K33" s="15"/>
     </row>
@@ -1399,10 +1399,10 @@
       <c r="K40" s="21"/>
     </row>
     <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="78" t="s">
+      <c r="B41" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="79"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="8">
         <v>3</v>
       </c>
@@ -1411,26 +1411,26 @@
       </c>
       <c r="F41" s="57"/>
       <c r="G41" s="35"/>
-      <c r="H41" s="78" t="s">
+      <c r="H41" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="79"/>
-      <c r="J41" s="8">
-        <v>6</v>
+      <c r="I41" s="67"/>
+      <c r="J41" s="36">
+        <v>5</v>
       </c>
       <c r="K41" s="14">
-        <v>2300</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="42" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="30"/>
       <c r="E42" s="29"/>
       <c r="F42" s="58"/>
       <c r="G42" s="35"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
       <c r="J42" s="30"/>
       <c r="K42" s="29"/>
     </row>
@@ -1467,7 +1467,7 @@
       <c r="I44" s="25"/>
       <c r="K44" s="14">
         <f>SUM(K41:K43)</f>
-        <v>2300</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -1481,14 +1481,14 @@
     <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="37" t="str">
         <f>H28</f>
-        <v>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</v>
+        <v>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="59"/>
       <c r="G46" s="35"/>
       <c r="H46" s="37" t="str">
         <f>B46</f>
-        <v>SEMANA  37        DEL    11     Al   17  SEPTIEMBRE    2023</v>
+        <v>SEMANA  38        DEL    18     Al   24  SEPTIEMBRE    2023</v>
       </c>
       <c r="K46" s="15"/>
     </row>
@@ -1502,23 +1502,23 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="67"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="73"/>
       <c r="F48" s="60"/>
       <c r="G48" s="35"/>
       <c r="H48" s="7"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="67"/>
+      <c r="J48" s="72"/>
+      <c r="K48" s="73"/>
     </row>
     <row r="49" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="69"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="75"/>
       <c r="F49" s="60"/>
       <c r="G49" s="35"/>
       <c r="H49" s="7"/>
-      <c r="J49" s="68"/>
-      <c r="K49" s="69"/>
+      <c r="J49" s="74"/>
+      <c r="K49" s="75"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="C51" s="27">
         <f ca="1">C33</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="59"/>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="I51" s="27">
         <f ca="1">I33</f>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="K51" s="15"/>
     </row>
@@ -1612,20 +1612,20 @@
       <c r="K57" s="43"/>
     </row>
     <row r="58" spans="2:11" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="78"/>
       <c r="D58" s="49"/>
       <c r="E58" s="45"/>
       <c r="J58" s="44"/>
       <c r="K58" s="45"/>
     </row>
     <row r="59" spans="2:11" s="35" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B59" s="70"/>
-      <c r="C59" s="70"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="79"/>
       <c r="D59" s="51"/>
       <c r="E59" s="52"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
       <c r="J59" s="41"/>
       <c r="K59" s="45"/>
     </row>
@@ -1634,8 +1634,8 @@
       <c r="C60" s="53"/>
       <c r="D60" s="54"/>
       <c r="E60" s="52"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
+      <c r="H60" s="81"/>
+      <c r="I60" s="81"/>
       <c r="J60" s="41"/>
       <c r="K60" s="46"/>
     </row>
@@ -1654,16 +1654,16 @@
     </row>
     <row r="64" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-      <c r="J65" s="71"/>
-      <c r="K65" s="71"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
+      <c r="J65" s="80"/>
+      <c r="K65" s="80"/>
     </row>
     <row r="66" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="71"/>
-      <c r="E66" s="71"/>
-      <c r="J66" s="71"/>
-      <c r="K66" s="71"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="J66" s="80"/>
+      <c r="K66" s="80"/>
     </row>
     <row r="67" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="2:11" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1676,11 +1676,13 @@
     <row r="70" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="J65:K66"/>
+    <mergeCell ref="H59:I60"/>
     <mergeCell ref="H5:I6"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H23:I23"/>
@@ -1689,13 +1691,11 @@
     <mergeCell ref="J11:K12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D30:E31"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="J48:K49"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="J65:K66"/>
-    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 20 OCT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -81,7 +81,7 @@
     <t>GUADALUPE LILLO TECOX</t>
   </si>
   <si>
-    <t>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</t>
+    <t>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</t>
   </si>
 </sst>
 </file>
@@ -531,21 +531,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -554,36 +584,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E55:E56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,7 @@
       <c r="H4" s="7"/>
       <c r="J4" s="36"/>
       <c r="K4" s="14">
-        <v>560</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -979,10 +979,10 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="70"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14">
         <v>0</v>
@@ -997,8 +997,8 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="72"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
       <c r="J6" s="13"/>
       <c r="K6" s="22">
         <v>0</v>
@@ -1016,7 +1016,7 @@
       <c r="H7" s="7"/>
       <c r="K7" s="39">
         <f>SUM(K4:K6)</f>
-        <v>560</v>
+        <v>840</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</v>
+        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -1047,30 +1047,30 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="16"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="70"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="72"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="77"/>
+      <c r="E13" s="74"/>
       <c r="F13" s="16"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="C14" s="27">
         <f ca="1">TODAY()</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="E14" s="15"/>
       <c r="G14" s="6"/>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="I14" s="27">
         <f ca="1">C14</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="K14" s="15"/>
     </row>
@@ -1186,10 +1186,10 @@
         <v>2800</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="75"/>
+      <c r="I23" s="64"/>
       <c r="J23" s="8">
         <v>6</v>
       </c>
@@ -1198,15 +1198,15 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="30"/>
       <c r="E24" s="29">
         <v>0</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
       <c r="J24" s="30"/>
       <c r="K24" s="29"/>
     </row>
@@ -1217,7 +1217,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="26">
-        <v>0</v>
+        <v>933</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="24"/>
@@ -1234,7 +1234,7 @@
       <c r="C26" s="25"/>
       <c r="E26" s="14">
         <f>SUM(E22:E25)</f>
-        <v>2800</v>
+        <v>3733</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="24"/>
@@ -1254,13 +1254,13 @@
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</v>
+        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
       </c>
       <c r="E28" s="15"/>
       <c r="G28" s="6"/>
       <c r="H28" s="37" t="str">
         <f>B28</f>
-        <v>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</v>
+        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
       </c>
       <c r="K28" s="15"/>
     </row>
@@ -1273,21 +1273,21 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="70"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="63"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="70"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="65"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="72"/>
       <c r="G31" s="6"/>
       <c r="H31" s="7"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="65"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="72"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="C33" s="27">
         <f ca="1">I14</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="E33" s="15"/>
       <c r="G33" s="6"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="I33" s="27">
         <f ca="1">C33</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="K33" s="15"/>
     </row>
@@ -1385,10 +1385,10 @@
       <c r="K40" s="21"/>
     </row>
     <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="74" t="s">
+      <c r="B41" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="75"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="8">
         <v>3</v>
       </c>
@@ -1397,10 +1397,10 @@
       </c>
       <c r="F41" s="57"/>
       <c r="G41" s="35"/>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="75"/>
+      <c r="I41" s="64"/>
       <c r="J41" s="36">
         <v>4</v>
       </c>
@@ -1409,14 +1409,14 @@
       </c>
     </row>
     <row r="42" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
       <c r="D42" s="30"/>
       <c r="E42" s="29"/>
       <c r="F42" s="58"/>
       <c r="G42" s="35"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
       <c r="J42" s="30"/>
       <c r="K42" s="29"/>
     </row>
@@ -1467,14 +1467,14 @@
     <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="37" t="str">
         <f>H28</f>
-        <v>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</v>
+        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="59"/>
       <c r="G46" s="35"/>
       <c r="H46" s="37" t="str">
         <f>B46</f>
-        <v>SEMANA  41        DEL    09     Al    15    OCTUBRE    2023</v>
+        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
       </c>
       <c r="K46" s="15"/>
     </row>
@@ -1488,23 +1488,23 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="63"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="70"/>
       <c r="F48" s="60"/>
       <c r="G48" s="35"/>
       <c r="H48" s="7"/>
-      <c r="J48" s="62"/>
-      <c r="K48" s="63"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="70"/>
     </row>
     <row r="49" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="65"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="72"/>
       <c r="F49" s="60"/>
       <c r="G49" s="35"/>
       <c r="H49" s="7"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="65"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="72"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="C51" s="27">
         <f ca="1">C33</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="59"/>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I51" s="27">
         <f ca="1">I33</f>
-        <v>45212</v>
+        <v>45219</v>
       </c>
       <c r="K51" s="15"/>
     </row>
@@ -1566,7 +1566,7 @@
       <c r="F53" s="34"/>
       <c r="G53" s="35"/>
       <c r="H53" s="35"/>
-      <c r="I53" s="78"/>
+      <c r="I53" s="61"/>
       <c r="J53" s="35"/>
       <c r="K53" s="35"/>
     </row>
@@ -1598,20 +1598,20 @@
       <c r="K57" s="43"/>
     </row>
     <row r="58" spans="2:11" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="61"/>
-      <c r="C58" s="61"/>
+      <c r="B58" s="75"/>
+      <c r="C58" s="75"/>
       <c r="D58" s="49"/>
       <c r="E58" s="45"/>
       <c r="J58" s="44"/>
       <c r="K58" s="45"/>
     </row>
     <row r="59" spans="2:11" s="35" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B59" s="66"/>
-      <c r="C59" s="66"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="76"/>
       <c r="D59" s="51"/>
       <c r="E59" s="52"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="68"/>
+      <c r="H59" s="78"/>
+      <c r="I59" s="78"/>
       <c r="J59" s="41"/>
       <c r="K59" s="45"/>
     </row>
@@ -1620,8 +1620,8 @@
       <c r="C60" s="53"/>
       <c r="D60" s="54"/>
       <c r="E60" s="52"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="68"/>
+      <c r="H60" s="78"/>
+      <c r="I60" s="78"/>
       <c r="J60" s="41"/>
       <c r="K60" s="46"/>
     </row>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="64" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="67"/>
-      <c r="E65" s="67"/>
-      <c r="J65" s="67"/>
-      <c r="K65" s="67"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
+      <c r="J65" s="77"/>
+      <c r="K65" s="77"/>
     </row>
     <row r="66" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="67"/>
-      <c r="E66" s="67"/>
-      <c r="J66" s="67"/>
-      <c r="K66" s="67"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="77"/>
+      <c r="J66" s="77"/>
+      <c r="K66" s="77"/>
     </row>
     <row r="67" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="2:11" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1662,11 +1662,13 @@
     <row r="70" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="J65:K66"/>
+    <mergeCell ref="H59:I60"/>
     <mergeCell ref="H5:I6"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H23:I23"/>
@@ -1675,13 +1677,11 @@
     <mergeCell ref="J11:K12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D30:E31"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="J48:K49"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="J65:K66"/>
-    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 27 OCT 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
+++ b/01 DOCUEMENTOS/RECIBOS NOMINA 2020.xlsx
@@ -81,7 +81,7 @@
     <t>GUADALUPE LILLO TECOX</t>
   </si>
   <si>
-    <t>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</t>
+    <t>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</t>
   </si>
 </sst>
 </file>
@@ -534,6 +534,42 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -543,47 +579,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -903,7 +903,7 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,7 @@
       <c r="H4" s="7"/>
       <c r="J4" s="36"/>
       <c r="K4" s="14">
-        <v>840</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -979,10 +979,10 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="66"/>
+      <c r="I5" s="71"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14">
         <v>0</v>
@@ -997,8 +997,8 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="68"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="73"/>
       <c r="J6" s="13"/>
       <c r="K6" s="22">
         <v>0</v>
@@ -1016,7 +1016,7 @@
       <c r="H7" s="7"/>
       <c r="K7" s="39">
         <f>SUM(K4:K6)</f>
-        <v>840</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
+        <v>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</v>
       </c>
       <c r="K9" s="15"/>
     </row>
@@ -1047,30 +1047,30 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
       <c r="F11" s="16"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="72"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="78"/>
       <c r="F13" s="16"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="C14" s="27">
         <f ca="1">TODAY()</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="E14" s="15"/>
       <c r="G14" s="6"/>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="I14" s="27">
         <f ca="1">C14</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="K14" s="15"/>
     </row>
@@ -1186,10 +1186,10 @@
         <v>2800</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="63" t="s">
+      <c r="H23" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="64"/>
+      <c r="I23" s="76"/>
       <c r="J23" s="8">
         <v>6</v>
       </c>
@@ -1198,15 +1198,15 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
       <c r="D24" s="30"/>
       <c r="E24" s="29">
         <v>0</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
       <c r="J24" s="30"/>
       <c r="K24" s="29"/>
     </row>
@@ -1217,7 +1217,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="26">
-        <v>933</v>
+        <v>0</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="24"/>
@@ -1234,7 +1234,7 @@
       <c r="C26" s="25"/>
       <c r="E26" s="14">
         <f>SUM(E22:E25)</f>
-        <v>3733</v>
+        <v>2800</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="24"/>
@@ -1254,13 +1254,13 @@
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="37" t="str">
         <f>B9</f>
-        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
+        <v>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</v>
       </c>
       <c r="E28" s="15"/>
       <c r="G28" s="6"/>
       <c r="H28" s="37" t="str">
         <f>B28</f>
-        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
+        <v>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</v>
       </c>
       <c r="K28" s="15"/>
     </row>
@@ -1273,21 +1273,21 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="70"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="70"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="64"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="72"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
       <c r="G31" s="6"/>
       <c r="H31" s="7"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="72"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="66"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="C33" s="27">
         <f ca="1">I14</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="E33" s="15"/>
       <c r="G33" s="6"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="I33" s="27">
         <f ca="1">C33</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="K33" s="15"/>
     </row>
@@ -1385,10 +1385,10 @@
       <c r="K40" s="21"/>
     </row>
     <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="64"/>
+      <c r="C41" s="76"/>
       <c r="D41" s="8">
         <v>3</v>
       </c>
@@ -1397,10 +1397,10 @@
       </c>
       <c r="F41" s="57"/>
       <c r="G41" s="35"/>
-      <c r="H41" s="63" t="s">
+      <c r="H41" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="64"/>
+      <c r="I41" s="76"/>
       <c r="J41" s="36">
         <v>4</v>
       </c>
@@ -1409,14 +1409,14 @@
       </c>
     </row>
     <row r="42" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
       <c r="D42" s="30"/>
       <c r="E42" s="29"/>
       <c r="F42" s="58"/>
       <c r="G42" s="35"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
       <c r="J42" s="30"/>
       <c r="K42" s="29"/>
     </row>
@@ -1467,14 +1467,14 @@
     <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="37" t="str">
         <f>H28</f>
-        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
+        <v>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="59"/>
       <c r="G46" s="35"/>
       <c r="H46" s="37" t="str">
         <f>B46</f>
-        <v>SEMANA  42        DEL    16     Al    22    OCTUBRE    2023</v>
+        <v>SEMANA  43        DEL    23     Al    29    OCTUBRE    2023</v>
       </c>
       <c r="K46" s="15"/>
     </row>
@@ -1488,23 +1488,23 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="70"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="64"/>
       <c r="F48" s="60"/>
       <c r="G48" s="35"/>
       <c r="H48" s="7"/>
-      <c r="J48" s="69"/>
-      <c r="K48" s="70"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="64"/>
     </row>
     <row r="49" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="72"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="66"/>
       <c r="F49" s="60"/>
       <c r="G49" s="35"/>
       <c r="H49" s="7"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="72"/>
+      <c r="J49" s="65"/>
+      <c r="K49" s="66"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="C51" s="27">
         <f ca="1">C33</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="59"/>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I51" s="27">
         <f ca="1">I33</f>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="K51" s="15"/>
     </row>
@@ -1598,20 +1598,20 @@
       <c r="K57" s="43"/>
     </row>
     <row r="58" spans="2:11" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="75"/>
-      <c r="C58" s="75"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
       <c r="D58" s="49"/>
       <c r="E58" s="45"/>
       <c r="J58" s="44"/>
       <c r="K58" s="45"/>
     </row>
     <row r="59" spans="2:11" s="35" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B59" s="76"/>
-      <c r="C59" s="76"/>
+      <c r="B59" s="67"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="51"/>
       <c r="E59" s="52"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="78"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
       <c r="J59" s="41"/>
       <c r="K59" s="45"/>
     </row>
@@ -1620,8 +1620,8 @@
       <c r="C60" s="53"/>
       <c r="D60" s="54"/>
       <c r="E60" s="52"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="78"/>
+      <c r="H60" s="69"/>
+      <c r="I60" s="69"/>
       <c r="J60" s="41"/>
       <c r="K60" s="46"/>
     </row>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="64" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="77"/>
-      <c r="E65" s="77"/>
-      <c r="J65" s="77"/>
-      <c r="K65" s="77"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="J65" s="68"/>
+      <c r="K65" s="68"/>
     </row>
     <row r="66" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="77"/>
-      <c r="E66" s="77"/>
-      <c r="J66" s="77"/>
-      <c r="K66" s="77"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="J66" s="68"/>
+      <c r="K66" s="68"/>
     </row>
     <row r="67" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="2:11" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1662,13 +1662,11 @@
     <row r="70" spans="2:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="J48:K49"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="J65:K66"/>
-    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="H5:I6"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H23:I23"/>
@@ -1677,11 +1675,13 @@
     <mergeCell ref="J11:K12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D30:E31"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="J65:K66"/>
+    <mergeCell ref="H59:I60"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="95" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>